<commit_message>
ipynb progress + ValueError: could not convert string to float:
</commit_message>
<xml_diff>
--- a/Trabalho 1 - Classificador/Dataset/dicionario_de_dados.xlsx
+++ b/Trabalho 1 - Classificador/Dataset/dicionario_de_dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\#ufrj_cursos_gravados\eel891_aprendizado_de_maquina\trabalhos\Trabalho1_Balanceado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\OneDrive\Documentos\GitHub\Introduction-to-Machine-Learning-EEL891\Trabalho 1 - Classificador\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEB0D33-63B1-4E8D-AE37-B46598AC66C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF53F43D-FB13-4F01-8C15-0C589D8E8FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conjunto de Treinamento" sheetId="2" r:id="rId1"/>
@@ -532,7 +532,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -700,6 +700,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -861,15 +873,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -929,9 +950,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -969,9 +990,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1004,26 +1025,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1056,26 +1060,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1252,22 +1239,22 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="94" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1284,7 +1271,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1301,7 +1288,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1318,7 +1305,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1332,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1342,11 +1329,11 @@
       <c r="C5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1360,7 +1347,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1370,14 +1357,14 @@
       <c r="C7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1388,7 +1375,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1405,7 +1392,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1419,7 +1406,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1436,7 +1423,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1450,7 +1437,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1460,14 +1447,14 @@
       <c r="C13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1477,11 +1464,11 @@
       <c r="C14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1491,11 +1478,11 @@
       <c r="C15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1512,7 +1499,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1529,7 +1516,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -1543,7 +1530,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -1553,14 +1540,14 @@
       <c r="C19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -1574,7 +1561,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -1588,7 +1575,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -1602,7 +1589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -1616,7 +1603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -1630,7 +1617,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -1644,7 +1631,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -1658,7 +1645,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -1672,7 +1659,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -1686,7 +1673,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -1703,7 +1690,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -1717,7 +1704,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -1731,7 +1718,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -1741,11 +1728,11 @@
       <c r="C32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -1755,14 +1742,14 @@
       <c r="C33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -1772,11 +1759,11 @@
       <c r="C34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -1793,7 +1780,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -1810,7 +1797,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -1827,7 +1814,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -1844,7 +1831,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -1861,7 +1848,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -1878,7 +1865,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -1892,7 +1879,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -1906,7 +1893,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -1937,18 +1924,18 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="84" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="94" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -1965,7 +1952,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1982,7 +1969,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1999,7 +1986,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2013,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2027,7 +2014,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2041,7 +2028,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2058,7 +2045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2069,7 +2056,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2086,7 +2073,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2100,7 +2087,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2117,7 +2104,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2131,7 +2118,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -2148,7 +2135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -2162,7 +2149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -2176,7 +2163,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -2193,7 +2180,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -2210,7 +2197,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -2224,7 +2211,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -2241,7 +2228,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -2255,7 +2242,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -2269,7 +2256,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -2283,7 +2270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -2297,7 +2284,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -2311,7 +2298,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -2325,7 +2312,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -2339,7 +2326,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2353,7 +2340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -2367,7 +2354,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -2384,7 +2371,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -2398,7 +2385,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -2412,7 +2399,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -2426,7 +2413,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -2443,7 +2430,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -2457,7 +2444,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -2474,7 +2461,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -2491,7 +2478,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -2508,7 +2495,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>36</v>
       </c>
@@ -2525,7 +2512,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -2542,7 +2529,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -2559,7 +2546,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -2573,7 +2560,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -2602,18 +2589,18 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="44" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="63.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="32.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="63.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -2630,7 +2617,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2647,7 +2634,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>

</xml_diff>